<commit_message>
Update link datasets - Corretta funzione link wiki
</commit_message>
<xml_diff>
--- a/_site/assets/datasets/1.xlsx
+++ b/_site/assets/datasets/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopopoletto/Google Drive/Sintesi C3—HATE SPEECH/Phase 02/z-SITO/Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edoardo/Google Drive/Sintesi C3—HATE SPEECH/Phase 02/z-SITO/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBA90C62-239F-464D-8AFC-B59DCEEDECBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2986D568-0707-3F4F-808B-ED3A899A1DB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="740" windowWidth="28200" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="740" windowWidth="28240" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hate speech_1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'hate speech_0'!$F$1:$F$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hate speech_1'!$F$1:$F$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hate speech_1'!$D$1:$E$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1684,7 +1677,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1692,13 +1685,13 @@
     <col min="1" max="1" width="8.33203125" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="47" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="52" customWidth="1"/>
-    <col min="8" max="8" width="41.5" style="39" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" customWidth="1"/>
-    <col min="10" max="10" width="34.83203125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="47" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="27" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="52" customWidth="1"/>
+    <col min="9" max="9" width="41.5" style="39" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1712,26 +1705,26 @@
       <c r="C1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>338</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>339</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>322</v>
       </c>
       <c r="K1" s="41" t="s">
         <v>336</v>
@@ -1748,27 +1741,27 @@
       <c r="C2" s="14">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" s="46">
         <f>((C2*100)-0.07) * ( (1000-1) / (($C$2*100)-0.07) ) + 1</f>
         <v>1000</v>
       </c>
-      <c r="E2" s="25">
+      <c r="G2" s="25">
         <v>2094</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G2" s="51">
+      <c r="H2" s="51">
         <v>1</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="J2" s="42" t="s">
-        <v>323</v>
       </c>
       <c r="K2" s="44">
         <v>5</v>
@@ -1785,27 +1778,27 @@
       <c r="C3" s="14">
         <v>5.5100000000000003E-2</v>
       </c>
-      <c r="D3" s="46">
-        <f t="shared" ref="D3:D66" si="1">((C3*100)-0.07) * ( (1000-1) / (($C$2*100)-0.07) ) + 1</f>
+      <c r="D3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="46">
+        <f t="shared" ref="F3:F66" si="1">((C3*100)-0.07) * ( (1000-1) / (($C$2*100)-0.07) ) + 1</f>
         <v>957.78873239436632</v>
       </c>
-      <c r="E3" s="25">
+      <c r="G3" s="25">
         <v>637</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="51">
+      <c r="H3" s="51">
         <v>4</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="I3" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K3" s="44">
         <v>2</v>
@@ -1822,27 +1815,27 @@
       <c r="C4" s="14">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" s="46">
         <f t="shared" si="1"/>
         <v>637.68661971831</v>
       </c>
-      <c r="E4" s="25">
+      <c r="G4" s="25">
         <v>33229</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G4" s="51">
+      <c r="H4" s="51">
         <v>1</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="I4" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>326</v>
       </c>
       <c r="K4" s="44">
         <v>6</v>
@@ -1859,27 +1852,27 @@
       <c r="C5" s="14">
         <v>0.03</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F5" s="46">
         <f t="shared" si="1"/>
         <v>516.32922535211276</v>
       </c>
-      <c r="E5" s="25">
+      <c r="G5" s="25">
         <v>220</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G5" s="51">
+      <c r="H5" s="51">
         <v>2</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="I5" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="J5" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K5" s="44">
         <v>2</v>
@@ -1896,27 +1889,27 @@
       <c r="C6" s="14">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6" s="46">
         <f t="shared" si="1"/>
         <v>428.3890845070423</v>
       </c>
-      <c r="E6" s="25">
+      <c r="G6" s="25">
         <v>1529</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>319</v>
-      </c>
-      <c r="G6" s="51">
+      <c r="H6" s="51">
         <v>5</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="I6" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="J6" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>326</v>
       </c>
       <c r="K6" s="44">
         <v>6</v>
@@ -1933,27 +1926,27 @@
       <c r="C7" s="14">
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F7" s="46">
         <f t="shared" si="1"/>
         <v>329.89612676056339</v>
       </c>
-      <c r="E7" s="25">
+      <c r="G7" s="25">
         <v>34244</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G7" s="51">
+      <c r="H7" s="51">
         <v>1</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="I7" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K7" s="44">
         <v>2</v>
@@ -1970,33 +1963,33 @@
       <c r="C8" s="14">
         <v>1.06E-2</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" s="46">
         <f t="shared" si="1"/>
         <v>175.12147887323945</v>
       </c>
-      <c r="E8" s="25">
+      <c r="G8" s="25">
         <v>809</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="51">
+      <c r="H8" s="51">
         <v>4</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="I8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K8" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A9" s="44">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2007,27 +2000,27 @@
       <c r="C9" s="14">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F9" s="46">
         <f t="shared" si="1"/>
         <v>136.42781690140848</v>
       </c>
-      <c r="E9" s="25">
+      <c r="G9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G9" s="51">
+      <c r="H9" s="51">
         <v>3</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="I9" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K9" s="44">
         <v>2</v>
@@ -2044,27 +2037,27 @@
       <c r="C10" s="14">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="46">
         <f t="shared" si="1"/>
         <v>90.698943661971839</v>
       </c>
-      <c r="E10" s="25">
+      <c r="G10" s="25">
         <v>1376</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="51">
+      <c r="H10" s="51">
         <v>4</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="I10" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K10" s="44">
         <v>2</v>
@@ -2081,27 +2074,27 @@
       <c r="C11" s="14">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F11" s="46">
         <f t="shared" si="1"/>
         <v>90.698943661971839</v>
       </c>
-      <c r="E11" s="25">
+      <c r="G11" s="25">
         <v>22240</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G11" s="51">
+      <c r="H11" s="51">
         <v>2</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K11" s="44">
         <v>2</v>
@@ -2118,27 +2111,27 @@
       <c r="C12" s="14">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F12" s="46">
         <f t="shared" si="1"/>
         <v>78.387323943661983</v>
       </c>
-      <c r="E12" s="25">
+      <c r="G12" s="25">
         <v>995</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G12" s="51">
+      <c r="H12" s="51">
         <v>2</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="I12" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="J12" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K12" s="44">
         <v>2</v>
@@ -2155,27 +2148,27 @@
       <c r="C13" s="14">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="F13" s="46">
         <f t="shared" si="1"/>
         <v>69.593309859154928</v>
       </c>
-      <c r="E13" s="25">
+      <c r="G13" s="25">
         <v>1385</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G13" s="51">
+      <c r="H13" s="51">
         <v>2</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="I13" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>76</v>
-      </c>
-      <c r="J13" s="42" t="s">
-        <v>329</v>
       </c>
       <c r="K13" s="44">
         <v>2</v>
@@ -2192,33 +2185,33 @@
       <c r="C14" s="14">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="F14" s="46">
         <f t="shared" si="1"/>
         <v>59.040492957746487</v>
       </c>
-      <c r="E14" s="25">
+      <c r="G14" s="25">
         <v>20.312999999999999</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G14" s="51">
+      <c r="H14" s="51">
         <v>1</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="I14" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="J14" s="42" t="s">
-        <v>329</v>
       </c>
       <c r="K14" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="255" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="44">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2229,27 +2222,27 @@
       <c r="C15" s="14">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="F15" s="46">
         <f t="shared" si="1"/>
         <v>57.281690140845065</v>
       </c>
-      <c r="E15" s="25">
+      <c r="G15" s="25">
         <v>88139</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="51">
+      <c r="H15" s="51">
         <v>4</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="I15" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="J15" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="J15" s="42" t="s">
-        <v>329</v>
       </c>
       <c r="K15" s="44">
         <v>2</v>
@@ -2266,25 +2259,25 @@
       <c r="C16" s="14">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F16" s="46">
         <f t="shared" si="1"/>
         <v>50.246478873239447</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G16" s="51">
+      <c r="G16" s="24"/>
+      <c r="H16" s="51">
         <v>1</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="I16" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="J16" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K16" s="44">
         <v>1</v>
@@ -2301,27 +2294,27 @@
       <c r="C17" s="14">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F17" s="46">
         <f t="shared" si="1"/>
         <v>48.487676056338024</v>
       </c>
-      <c r="E17" s="25">
+      <c r="G17" s="25">
         <v>11</v>
       </c>
-      <c r="F17" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G17" s="51">
+      <c r="H17" s="51">
         <v>3</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="I17" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="J17" s="15" t="s">
         <v>91</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K17" s="44">
         <v>2</v>
@@ -2338,27 +2331,27 @@
       <c r="C18" s="14">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F18" s="46">
         <f t="shared" si="1"/>
         <v>43.211267605633807</v>
       </c>
-      <c r="E18" s="25">
+      <c r="G18" s="25">
         <v>148</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G18" s="51">
+      <c r="H18" s="51">
         <v>2</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="I18" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="J18" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="J18" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K18" s="44">
         <v>2</v>
@@ -2375,27 +2368,27 @@
       <c r="C19" s="14">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D19" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="F19" s="46">
         <f t="shared" si="1"/>
         <v>43.211267605633807</v>
       </c>
-      <c r="E19" s="25">
+      <c r="G19" s="25">
         <v>479</v>
       </c>
-      <c r="F19" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G19" s="51">
+      <c r="H19" s="51">
         <v>1</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="I19" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="J19" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>328</v>
       </c>
       <c r="K19" s="44">
         <v>4</v>
@@ -2412,27 +2405,27 @@
       <c r="C20" s="14">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F20" s="46">
         <f t="shared" si="1"/>
         <v>39.693661971830984</v>
       </c>
-      <c r="E20" s="25">
+      <c r="G20" s="25">
         <v>120</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G20" s="51">
+      <c r="H20" s="51">
         <v>2</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="I20" s="33" t="s">
         <v>325</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="J20" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>326</v>
       </c>
       <c r="K20" s="44">
         <v>6</v>
@@ -2449,27 +2442,27 @@
       <c r="C21" s="14">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D21" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F21" s="46">
         <f t="shared" si="1"/>
         <v>39.693661971830984</v>
       </c>
-      <c r="E21" s="25">
+      <c r="G21" s="25">
         <v>18981</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G21" s="51">
+      <c r="H21" s="51">
         <v>1</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="I21" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="J21" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K21" s="44">
         <v>2</v>
@@ -2486,27 +2479,27 @@
       <c r="C22" s="14">
         <v>2.8E-3</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F22" s="46">
         <f t="shared" si="1"/>
         <v>37.934859154929576</v>
       </c>
-      <c r="E22" s="25">
+      <c r="G22" s="25">
         <v>20859</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="G22" s="51">
+      <c r="H22" s="51">
         <v>6</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="I22" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="J22" s="20" t="s">
         <v>105</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K22" s="44">
         <v>2</v>
@@ -2523,27 +2516,27 @@
       <c r="C23" s="14">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F23" s="46">
         <f t="shared" si="1"/>
         <v>34.417253521126767</v>
       </c>
-      <c r="E23" s="25">
+      <c r="G23" s="25">
         <v>28678</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G23" s="51">
+      <c r="H23" s="51">
         <v>1</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="I23" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="J23" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K23" s="44">
         <v>2</v>
@@ -2560,27 +2553,27 @@
       <c r="C24" s="14">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="D24" s="46">
+      <c r="D24" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F24" s="46">
         <f t="shared" si="1"/>
         <v>34.417253521126767</v>
       </c>
-      <c r="E24" s="25">
+      <c r="G24" s="25">
         <v>718</v>
       </c>
-      <c r="F24" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G24" s="51">
+      <c r="H24" s="51">
         <v>2</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="I24" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="J24" s="20" t="s">
         <v>114</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>327</v>
       </c>
       <c r="K24" s="44">
         <v>3</v>
@@ -2597,27 +2590,27 @@
       <c r="C25" s="14">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F25" s="46">
         <f t="shared" si="1"/>
         <v>30.899647887323944</v>
       </c>
-      <c r="E25" s="25">
+      <c r="G25" s="25">
         <v>1216</v>
       </c>
-      <c r="F25" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="G25" s="51">
+      <c r="H25" s="51">
         <v>2</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="I25" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="J25" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K25" s="44">
         <v>1</v>
@@ -2634,27 +2627,27 @@
       <c r="C26" s="14">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="D26" s="46">
+      <c r="D26" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F26" s="46">
         <f t="shared" si="1"/>
         <v>25.62323943661972</v>
       </c>
-      <c r="E26" s="25">
+      <c r="G26" s="25">
         <v>4739</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="G26" s="51">
+      <c r="H26" s="51">
         <v>2</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="I26" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="I26" s="20" t="s">
+      <c r="J26" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K26" s="44">
         <v>2</v>
@@ -2671,27 +2664,27 @@
       <c r="C27" s="14">
         <v>2E-3</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D27" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F27" s="46">
         <f t="shared" si="1"/>
         <v>23.864436619718312</v>
       </c>
-      <c r="E27" s="25">
+      <c r="G27" s="25">
         <v>37793</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G27" s="51">
+      <c r="H27" s="51">
         <v>1</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="I27" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="J27" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>327</v>
       </c>
       <c r="K27" s="44">
         <v>3</v>
@@ -2708,33 +2701,33 @@
       <c r="C28" s="14">
         <v>2E-3</v>
       </c>
-      <c r="D28" s="46">
+      <c r="D28" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F28" s="46">
         <f t="shared" si="1"/>
         <v>23.864436619718312</v>
       </c>
-      <c r="E28" s="25">
+      <c r="G28" s="25">
         <v>337</v>
       </c>
-      <c r="F28" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G28" s="51">
+      <c r="H28" s="51">
         <v>2</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="I28" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="J28" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K28" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="44">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2745,27 +2738,27 @@
       <c r="C29" s="14">
         <v>1.9E-3</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F29" s="46">
         <f t="shared" si="1"/>
         <v>22.105633802816904</v>
       </c>
-      <c r="E29" s="25">
+      <c r="G29" s="25">
         <v>425</v>
       </c>
-      <c r="F29" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="51">
+      <c r="H29" s="51">
         <v>4</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="I29" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="J29" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K29" s="44">
         <v>1</v>
@@ -2782,27 +2775,27 @@
       <c r="C30" s="14">
         <v>1.8E-3</v>
       </c>
-      <c r="D30" s="46">
+      <c r="D30" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F30" s="46">
         <f t="shared" si="1"/>
         <v>20.346830985915492</v>
       </c>
-      <c r="E30" s="25">
+      <c r="G30" s="25">
         <v>6</v>
       </c>
-      <c r="F30" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G30" s="51">
+      <c r="H30" s="51">
         <v>3</v>
       </c>
-      <c r="H30" s="33" t="s">
+      <c r="I30" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="20" t="s">
+      <c r="J30" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K30" s="44">
         <v>2</v>
@@ -2819,33 +2812,33 @@
       <c r="C31" s="14">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D31" s="46">
+      <c r="D31" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F31" s="46">
         <f t="shared" si="1"/>
         <v>18.588028169014084</v>
       </c>
-      <c r="E31" s="25">
+      <c r="G31" s="25">
         <v>1455</v>
       </c>
-      <c r="F31" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G31" s="51">
+      <c r="H31" s="51">
         <v>2</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="I31" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="J31" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="J31" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K31" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="221" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2856,27 +2849,27 @@
       <c r="C32" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D32" s="46">
+      <c r="D32" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F32" s="46">
         <f t="shared" si="1"/>
         <v>16.82922535211268</v>
       </c>
-      <c r="E32" s="25">
+      <c r="G32" s="25">
         <v>1765</v>
       </c>
-      <c r="F32" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G32" s="51">
+      <c r="H32" s="51">
         <v>2</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="I32" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="J32" s="15" t="s">
         <v>141</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K32" s="44">
         <v>2</v>
@@ -2893,27 +2886,27 @@
       <c r="C33" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D33" s="46">
+      <c r="D33" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F33" s="46">
         <f t="shared" si="1"/>
         <v>16.82922535211268</v>
       </c>
-      <c r="E33" s="25">
+      <c r="G33" s="25">
         <v>107</v>
       </c>
-      <c r="F33" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G33" s="51">
+      <c r="H33" s="51">
         <v>2</v>
       </c>
-      <c r="H33" s="33" t="s">
+      <c r="I33" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="J33" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="J33" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K33" s="44">
         <v>2</v>
@@ -2930,27 +2923,27 @@
       <c r="C34" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D34" s="46">
+      <c r="D34" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="F34" s="46">
         <f t="shared" si="1"/>
         <v>16.82922535211268</v>
       </c>
-      <c r="E34" s="25">
+      <c r="G34" s="25">
         <v>57887</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G34" s="51">
+      <c r="H34" s="51">
         <v>1</v>
       </c>
-      <c r="H34" s="33" t="s">
+      <c r="I34" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="I34" s="20" t="s">
+      <c r="J34" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="J34" s="29" t="s">
-        <v>335</v>
       </c>
       <c r="K34" s="44">
         <v>7</v>
@@ -2967,27 +2960,27 @@
       <c r="C35" s="14">
         <v>1.5E-3</v>
       </c>
-      <c r="D35" s="46">
+      <c r="D35" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F35" s="46">
         <f t="shared" si="1"/>
         <v>15.070422535211266</v>
       </c>
-      <c r="E35" s="25">
+      <c r="G35" s="25">
         <v>1178</v>
       </c>
-      <c r="F35" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G35" s="51">
+      <c r="H35" s="51">
         <v>2</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="I35" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="J35" s="20" t="s">
         <v>152</v>
-      </c>
-      <c r="J35" s="29" t="s">
-        <v>327</v>
       </c>
       <c r="K35" s="44">
         <v>3</v>
@@ -3004,27 +2997,27 @@
       <c r="C36" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="D36" s="46">
+      <c r="D36" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F36" s="46">
         <f t="shared" si="1"/>
         <v>13.311619718309856</v>
       </c>
-      <c r="E36" s="25">
+      <c r="G36" s="25">
         <v>554008</v>
       </c>
-      <c r="F36" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G36" s="51">
+      <c r="H36" s="51">
         <v>2</v>
       </c>
-      <c r="H36" s="33" t="s">
+      <c r="I36" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="J36" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K36" s="44">
         <v>2</v>
@@ -3041,27 +3034,27 @@
       <c r="C37" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="46">
         <f t="shared" si="1"/>
         <v>13.311619718309856</v>
       </c>
-      <c r="E37" s="25">
+      <c r="G37" s="25">
         <v>5519</v>
       </c>
-      <c r="F37" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G37" s="51">
+      <c r="H37" s="51">
         <v>1</v>
       </c>
-      <c r="H37" s="33" t="s">
+      <c r="I37" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K37" s="44">
         <v>2</v>
@@ -3078,27 +3071,27 @@
       <c r="C38" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="D38" s="46">
+      <c r="D38" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F38" s="46">
         <f t="shared" si="1"/>
         <v>13.311619718309856</v>
       </c>
-      <c r="E38" s="25">
+      <c r="G38" s="25">
         <v>1718</v>
       </c>
-      <c r="F38" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="51">
+      <c r="H38" s="51">
         <v>4</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="I38" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="J38" s="15" t="s">
         <v>161</v>
-      </c>
-      <c r="J38" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K38" s="44">
         <v>1</v>
@@ -3115,27 +3108,27 @@
       <c r="C39" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="D39" s="46">
+      <c r="D39" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F39" s="46">
         <f t="shared" si="1"/>
         <v>13.311619718309856</v>
       </c>
-      <c r="E39" s="25">
+      <c r="G39" s="25">
         <v>837</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G39" s="51">
+      <c r="H39" s="51">
         <v>2</v>
       </c>
-      <c r="H39" s="33" t="s">
+      <c r="I39" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K39" s="44">
         <v>1</v>
@@ -3152,27 +3145,27 @@
       <c r="C40" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D40" s="46">
+      <c r="D40" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F40" s="46">
         <f t="shared" si="1"/>
         <v>11.552816901408452</v>
       </c>
-      <c r="E40" s="25">
+      <c r="G40" s="25">
         <v>342234</v>
       </c>
-      <c r="F40" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G40" s="51">
+      <c r="H40" s="51">
         <v>1</v>
       </c>
-      <c r="H40" s="33" t="s">
+      <c r="I40" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="J40" s="20" t="s">
         <v>167</v>
-      </c>
-      <c r="J40" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K40" s="44">
         <v>2</v>
@@ -3189,27 +3182,27 @@
       <c r="C41" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D41" s="46">
+      <c r="D41" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F41" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E41" s="25">
+      <c r="G41" s="25">
         <v>920</v>
       </c>
-      <c r="F41" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G41" s="51">
+      <c r="H41" s="51">
         <v>2</v>
       </c>
-      <c r="H41" s="33" t="s">
+      <c r="I41" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="J41" s="20" t="s">
         <v>180</v>
-      </c>
-      <c r="J41" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K41" s="44">
         <v>2</v>
@@ -3226,33 +3219,33 @@
       <c r="C42" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F42" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E42" s="25">
+      <c r="G42" s="25">
         <v>578</v>
       </c>
-      <c r="F42" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="51">
+      <c r="H42" s="51">
         <v>4</v>
       </c>
-      <c r="H42" s="33" t="s">
+      <c r="I42" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="I42" s="20" t="s">
+      <c r="J42" s="20" t="s">
         <v>184</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K42" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="238" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A43" s="44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3263,27 +3256,27 @@
       <c r="C43" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D43" s="46">
+      <c r="D43" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="F43" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E43" s="25">
+      <c r="G43" s="25">
         <v>3248</v>
       </c>
-      <c r="F43" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G43" s="51">
+      <c r="H43" s="51">
         <v>2</v>
       </c>
-      <c r="H43" s="33" t="s">
+      <c r="I43" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="I43" s="20" t="s">
+      <c r="J43" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="J43" s="29" t="s">
-        <v>335</v>
       </c>
       <c r="K43" s="44">
         <v>7</v>
@@ -3300,27 +3293,27 @@
       <c r="C44" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D44" s="46">
+      <c r="D44" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F44" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E44" s="25">
+      <c r="G44" s="25">
         <v>409894</v>
       </c>
-      <c r="F44" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G44" s="51">
+      <c r="H44" s="51">
         <v>1</v>
       </c>
-      <c r="H44" s="33" t="s">
+      <c r="I44" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="J44" s="15" t="s">
         <v>191</v>
-      </c>
-      <c r="J44" s="29" t="s">
-        <v>323</v>
       </c>
       <c r="K44" s="44">
         <v>5</v>
@@ -3337,27 +3330,27 @@
       <c r="C45" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D45" s="46">
+      <c r="D45" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F45" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E45" s="25">
+      <c r="G45" s="25">
         <v>2017</v>
       </c>
-      <c r="F45" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G45" s="51">
+      <c r="H45" s="51">
         <v>1</v>
       </c>
-      <c r="H45" s="33" t="s">
+      <c r="I45" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="J45" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K45" s="44">
         <v>2</v>
@@ -3374,27 +3367,27 @@
       <c r="C46" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D46" s="46">
+      <c r="D46" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F46" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E46" s="25">
+      <c r="G46" s="25">
         <v>1542569</v>
       </c>
-      <c r="F46" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G46" s="51">
+      <c r="H46" s="51">
         <v>1</v>
       </c>
-      <c r="H46" s="33" t="s">
+      <c r="I46" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="I46" s="20" t="s">
+      <c r="J46" s="20" t="s">
         <v>199</v>
-      </c>
-      <c r="J46" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K46" s="44">
         <v>1</v>
@@ -3411,27 +3404,27 @@
       <c r="C47" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D47" s="46">
+      <c r="D47" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F47" s="46">
         <f t="shared" si="1"/>
         <v>9.794014084507042</v>
       </c>
-      <c r="E47" s="25">
+      <c r="G47" s="25">
         <v>602</v>
       </c>
-      <c r="F47" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G47" s="51">
+      <c r="H47" s="51">
         <v>2</v>
       </c>
-      <c r="H47" s="33" t="s">
+      <c r="I47" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="J47" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="J47" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K47" s="44">
         <v>2</v>
@@ -3448,27 +3441,27 @@
       <c r="C48" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D48" s="46">
+      <c r="D48" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F48" s="46">
         <f t="shared" si="1"/>
         <v>8.0352112676056322</v>
       </c>
-      <c r="E48" s="25">
+      <c r="G48" s="25">
         <v>7928</v>
       </c>
-      <c r="F48" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G48" s="51">
+      <c r="H48" s="51">
         <v>2</v>
       </c>
-      <c r="H48" s="33" t="s">
+      <c r="I48" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="I48" s="20" t="s">
+      <c r="J48" s="20" t="s">
         <v>206</v>
-      </c>
-      <c r="J48" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K48" s="44">
         <v>2</v>
@@ -3485,27 +3478,27 @@
       <c r="C49" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D49" s="46">
+      <c r="D49" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F49" s="46">
         <f t="shared" si="1"/>
         <v>8.0352112676056322</v>
       </c>
-      <c r="E49" s="25">
+      <c r="G49" s="25">
         <v>46876</v>
       </c>
-      <c r="F49" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G49" s="51">
+      <c r="H49" s="51">
         <v>1</v>
       </c>
-      <c r="H49" s="33" t="s">
+      <c r="I49" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="I49" s="20" t="s">
+      <c r="J49" s="20" t="s">
         <v>209</v>
-      </c>
-      <c r="J49" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K49" s="44">
         <v>2</v>
@@ -3522,33 +3515,33 @@
       <c r="C50" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D50" s="46">
+      <c r="D50" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F50" s="46">
         <f t="shared" si="1"/>
         <v>6.2764084507042259</v>
       </c>
-      <c r="E50" s="25">
+      <c r="G50" s="25">
         <v>457</v>
       </c>
-      <c r="F50" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G50" s="51">
+      <c r="H50" s="51">
         <v>2</v>
       </c>
-      <c r="H50" s="33" t="s">
+      <c r="I50" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="I50" s="20" t="s">
+      <c r="J50" s="20" t="s">
         <v>210</v>
-      </c>
-      <c r="J50" s="29" t="s">
-        <v>326</v>
       </c>
       <c r="K50" s="44">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3559,33 +3552,33 @@
       <c r="C51" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D51" s="46">
+      <c r="D51" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F51" s="46">
         <f t="shared" si="1"/>
         <v>6.2764084507042259</v>
       </c>
-      <c r="E51" s="25">
+      <c r="G51" s="25">
         <v>1</v>
       </c>
-      <c r="F51" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G51" s="51">
+      <c r="H51" s="51">
         <v>3</v>
       </c>
-      <c r="H51" s="33" t="s">
+      <c r="I51" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="J51" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K51" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3596,33 +3589,33 @@
       <c r="C52" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D52" s="46">
+      <c r="D52" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F52" s="46">
         <f t="shared" si="1"/>
         <v>6.2764084507042259</v>
       </c>
-      <c r="E52" s="25">
+      <c r="G52" s="25">
         <v>5266</v>
       </c>
-      <c r="F52" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G52" s="51">
+      <c r="H52" s="51">
         <v>2</v>
       </c>
-      <c r="H52" s="33" t="s">
+      <c r="I52" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="J52" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="J52" s="29" t="s">
-        <v>327</v>
       </c>
       <c r="K52" s="44">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3633,27 +3626,27 @@
       <c r="C53" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D53" s="46">
+      <c r="D53" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F53" s="46">
         <f t="shared" si="1"/>
         <v>6.2764084507042259</v>
       </c>
-      <c r="E53" s="25">
+      <c r="G53" s="25">
         <v>229</v>
       </c>
-      <c r="F53" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G53" s="51">
+      <c r="H53" s="51">
         <v>3</v>
       </c>
-      <c r="H53" s="33" t="s">
+      <c r="I53" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="J53" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="J53" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K53" s="44">
         <v>2</v>
@@ -3670,27 +3663,27 @@
       <c r="C54" s="14">
         <v>1E-3</v>
       </c>
-      <c r="D54" s="46">
+      <c r="D54" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F54" s="46">
         <f t="shared" si="1"/>
         <v>6.2764084507042259</v>
       </c>
-      <c r="E54" s="25">
+      <c r="G54" s="25">
         <v>2490</v>
       </c>
-      <c r="F54" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54" s="51">
+      <c r="H54" s="51">
         <v>4</v>
       </c>
-      <c r="H54" s="33" t="s">
+      <c r="I54" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="J54" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="J54" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K54" s="44">
         <v>2</v>
@@ -3707,33 +3700,33 @@
       <c r="C55" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D55" s="46">
+      <c r="D55" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F55" s="46">
         <f t="shared" si="1"/>
         <v>4.5176056338028161</v>
       </c>
-      <c r="E55" s="25">
+      <c r="G55" s="25">
         <v>104</v>
       </c>
-      <c r="F55" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G55" s="51">
+      <c r="H55" s="51">
         <v>2</v>
       </c>
-      <c r="H55" s="33" t="s">
+      <c r="I55" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="J55" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="J55" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K55" s="44">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A56" s="44">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3744,27 +3737,27 @@
       <c r="C56" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D56" s="46">
+      <c r="D56" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F56" s="46">
         <f t="shared" si="1"/>
         <v>4.5176056338028161</v>
       </c>
-      <c r="E56" s="25">
+      <c r="G56" s="25">
         <v>69</v>
       </c>
-      <c r="F56" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G56" s="51">
+      <c r="H56" s="51">
         <v>3</v>
       </c>
-      <c r="H56" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I56" s="5" t="s">
+      <c r="J56" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="J56" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K56" s="44">
         <v>2</v>
@@ -3781,27 +3774,27 @@
       <c r="C57" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D57" s="46">
+      <c r="D57" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F57" s="46">
         <f t="shared" si="1"/>
         <v>4.5176056338028161</v>
       </c>
-      <c r="E57" s="25">
+      <c r="G57" s="25">
         <v>3</v>
       </c>
-      <c r="F57" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G57" s="51">
+      <c r="H57" s="51">
         <v>3</v>
       </c>
-      <c r="H57" s="33" t="s">
+      <c r="I57" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="I57" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="J57" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K57" s="44">
         <v>2</v>
@@ -3818,27 +3811,27 @@
       <c r="C58" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D58" s="46">
+      <c r="D58" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F58" s="46">
         <f t="shared" si="1"/>
         <v>4.5176056338028161</v>
       </c>
-      <c r="E58" s="25">
+      <c r="G58" s="25">
         <v>504</v>
       </c>
-      <c r="F58" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G58" s="51">
+      <c r="H58" s="51">
         <v>2</v>
       </c>
-      <c r="H58" s="33" t="s">
+      <c r="I58" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="J58" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="J58" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K58" s="44">
         <v>2</v>
@@ -3855,27 +3848,27 @@
       <c r="C59" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D59" s="46">
+      <c r="D59" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F59" s="46">
         <f t="shared" si="1"/>
         <v>2.7588028169014081</v>
       </c>
-      <c r="E59" s="25">
+      <c r="G59" s="25">
         <v>1002047</v>
       </c>
-      <c r="F59" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G59" s="51">
+      <c r="H59" s="51">
         <v>2</v>
       </c>
-      <c r="H59" s="33" t="s">
+      <c r="I59" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="I59" s="20" t="s">
+      <c r="J59" s="20" t="s">
         <v>231</v>
-      </c>
-      <c r="J59" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K59" s="44">
         <v>2</v>
@@ -3892,33 +3885,33 @@
       <c r="C60" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D60" s="46">
+      <c r="D60" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="F60" s="46">
         <f t="shared" si="1"/>
         <v>2.7588028169014081</v>
       </c>
-      <c r="E60" s="25">
+      <c r="G60" s="25">
         <v>1252</v>
       </c>
-      <c r="F60" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G60" s="51">
+      <c r="H60" s="51">
         <v>2</v>
       </c>
-      <c r="H60" s="33" t="s">
+      <c r="I60" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="I60" s="20" t="s">
+      <c r="J60" s="20" t="s">
         <v>234</v>
-      </c>
-      <c r="J60" s="29" t="s">
-        <v>328</v>
       </c>
       <c r="K60" s="44">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3929,27 +3922,27 @@
       <c r="C61" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D61" s="46">
+      <c r="D61" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F61" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E61" s="25">
+      <c r="G61" s="25">
         <v>322</v>
       </c>
-      <c r="F61" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="G61" s="51">
+      <c r="H61" s="51">
         <v>3</v>
       </c>
-      <c r="H61" s="33" t="s">
+      <c r="I61" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I61" s="20" t="s">
+      <c r="J61" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="J61" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K61" s="44">
         <v>2</v>
@@ -3966,27 +3959,27 @@
       <c r="C62" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D62" s="46">
+      <c r="D62" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F62" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E62" s="25">
+      <c r="G62" s="25">
         <v>2589478</v>
       </c>
-      <c r="F62" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="G62" s="51">
+      <c r="H62" s="51">
         <v>1</v>
       </c>
-      <c r="H62" s="33" t="s">
+      <c r="I62" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="I62" s="20" t="s">
+      <c r="J62" s="20" t="s">
         <v>238</v>
-      </c>
-      <c r="J62" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K62" s="44">
         <v>2</v>
@@ -4003,27 +3996,27 @@
       <c r="C63" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D63" s="46">
+      <c r="D63" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F63" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E63" s="25">
+      <c r="G63" s="25">
         <v>14.635</v>
       </c>
-      <c r="F63" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G63" s="51">
+      <c r="H63" s="51">
         <v>2</v>
       </c>
-      <c r="H63" s="33" t="s">
+      <c r="I63" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="I63" s="20" t="s">
+      <c r="J63" s="20" t="s">
         <v>241</v>
-      </c>
-      <c r="J63" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K63" s="44">
         <v>1</v>
@@ -4040,27 +4033,27 @@
       <c r="C64" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D64" s="46">
+      <c r="D64" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F64" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E64" s="25">
+      <c r="G64" s="25">
         <v>1.6459999999999999</v>
       </c>
-      <c r="F64" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="51">
+      <c r="H64" s="51">
         <v>4</v>
       </c>
-      <c r="H64" s="33" t="s">
+      <c r="I64" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="I64" s="20" t="s">
+      <c r="J64" s="20" t="s">
         <v>243</v>
-      </c>
-      <c r="J64" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K64" s="44">
         <v>1</v>
@@ -4077,27 +4070,27 @@
       <c r="C65" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D65" s="46">
+      <c r="D65" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F65" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E65" s="25">
+      <c r="G65" s="25">
         <v>102</v>
       </c>
-      <c r="F65" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G65" s="51">
+      <c r="H65" s="51">
         <v>2</v>
       </c>
-      <c r="H65" s="33" t="s">
+      <c r="I65" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="I65" s="20" t="s">
+      <c r="J65" s="20" t="s">
         <v>246</v>
-      </c>
-      <c r="J65" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="K65" s="44">
         <v>1</v>
@@ -4114,27 +4107,27 @@
       <c r="C66" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D66" s="46">
+      <c r="D66" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F66" s="46">
         <f t="shared" si="1"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E66" s="25">
+      <c r="G66" s="25">
         <v>14.637</v>
       </c>
-      <c r="F66" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G66" s="51">
+      <c r="H66" s="51">
         <v>4</v>
       </c>
-      <c r="H66" s="33" t="s">
+      <c r="I66" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="I66" s="20" t="s">
+      <c r="J66" s="20" t="s">
         <v>218</v>
-      </c>
-      <c r="J66" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K66" s="44">
         <v>2</v>
@@ -4151,27 +4144,27 @@
       <c r="C67" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D67" s="46">
-        <f t="shared" ref="D67:D68" si="3">((C67*100)-0.07) * ( (1000-1) / (($C$2*100)-0.07) ) + 1</f>
+      <c r="D67" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="F67" s="46">
+        <f t="shared" ref="F67:F68" si="3">((C67*100)-0.07) * ( (1000-1) / (($C$2*100)-0.07) ) + 1</f>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E67" s="25">
+      <c r="G67" s="25">
         <v>456</v>
       </c>
-      <c r="F67" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G67" s="51">
+      <c r="H67" s="51">
         <v>2</v>
       </c>
-      <c r="H67" s="33" t="s">
+      <c r="I67" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="I67" s="20" t="s">
+      <c r="J67" s="20" t="s">
         <v>250</v>
-      </c>
-      <c r="J67" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="K67" s="44">
         <v>2</v>
@@ -4188,91 +4181,90 @@
       <c r="C68" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D68" s="46">
+      <c r="D68" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F68" s="46">
         <f t="shared" si="3"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="E68" s="25">
+      <c r="G68" s="25">
         <v>231</v>
       </c>
-      <c r="F68" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="G68" s="51">
+      <c r="H68" s="51">
         <v>2</v>
       </c>
-      <c r="H68" s="33" t="s">
+      <c r="I68" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="I68" s="15" t="s">
+      <c r="J68" s="15" t="s">
         <v>253</v>
-      </c>
-      <c r="J68" s="29" t="s">
-        <v>326</v>
       </c>
       <c r="K68" s="44">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F68" xr:uid="{993D185A-3C58-664E-A59B-469E971A35A3}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="I8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="I9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="B10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="I10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="I11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="I12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="I13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="I15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="B16" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="I16" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="I17" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="I18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J16" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J17" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="J18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="B19" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="I19" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J19" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="B20" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="I20" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="J20" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="B21" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="B22" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="I22" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="J22" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="B23" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="B24" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="B27" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="I27" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="J27" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
     <hyperlink ref="B28" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="I28" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="I29" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="I30" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="I31" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="J28" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="J29" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="J30" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="J31" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="B32" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="I32" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="J32" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="B33" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="I33" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="J33" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="B35" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="B38" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="I38" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="J38" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="B39" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
     <hyperlink ref="B40" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
     <hyperlink ref="B41" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="B42" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="B43" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="B44" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="I44" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="J44" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
     <hyperlink ref="B45" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
     <hyperlink ref="B47" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="B48" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
@@ -4289,31 +4281,31 @@
     <hyperlink ref="B65" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
     <hyperlink ref="B66" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
     <hyperlink ref="B67" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="I68" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="I21" r:id="rId74" xr:uid="{83A801EE-E546-7444-83B0-7AE4FE5DCC18}"/>
-    <hyperlink ref="I23" r:id="rId75" xr:uid="{6B290F46-1AB5-9544-B3B3-FCE151FC026C}"/>
-    <hyperlink ref="I24" r:id="rId76" xr:uid="{930265A3-4A43-114B-89F7-0D260397ECEE}"/>
-    <hyperlink ref="I25" r:id="rId77" xr:uid="{D7F1F70C-9733-5E46-8B18-FE50DAF1E02B}"/>
-    <hyperlink ref="I26" r:id="rId78" xr:uid="{65733835-2CD9-5749-BBDD-3CBBC33C96FA}"/>
-    <hyperlink ref="I34" r:id="rId79" xr:uid="{5C774A6A-9EAA-6A41-B786-2F3DEE421DF6}"/>
-    <hyperlink ref="I35" r:id="rId80" xr:uid="{1AFAE886-D23A-4C44-9377-F08511F4CB51}"/>
-    <hyperlink ref="I40" r:id="rId81" xr:uid="{04363683-E801-4A40-92D4-F5E22A223193}"/>
-    <hyperlink ref="I41" r:id="rId82" xr:uid="{7765E9B8-43EB-BB45-91B0-4FF8F7D8E3BD}"/>
-    <hyperlink ref="I43" r:id="rId83" xr:uid="{BB0F6366-7063-134D-8A4B-076195A1E08F}"/>
-    <hyperlink ref="I42" r:id="rId84" xr:uid="{DE89AC9B-B4B6-4144-B0BA-3DECB15EAEA2}"/>
-    <hyperlink ref="I46" r:id="rId85" xr:uid="{824B515C-AA87-F043-A139-784BCBF016E6}"/>
-    <hyperlink ref="I49" r:id="rId86" xr:uid="{2AF4CA48-6D36-5947-991C-981DDFA018C7}"/>
-    <hyperlink ref="I50" r:id="rId87" xr:uid="{7056C87E-C05C-9E40-A22A-461D400945D8}"/>
-    <hyperlink ref="I48" r:id="rId88" xr:uid="{7BFDE7F6-5EE7-DB44-9A8C-4A94BA0E0D34}"/>
-    <hyperlink ref="I59" r:id="rId89" xr:uid="{4FE03561-7F01-C941-B63F-6A1C5611F8E0}"/>
-    <hyperlink ref="I60" r:id="rId90" xr:uid="{3EBD3D55-540B-4C48-B378-A997181200FD}"/>
-    <hyperlink ref="I62" r:id="rId91" xr:uid="{3EA893CD-E3C9-F04E-B2E2-7E1A74D042FC}"/>
-    <hyperlink ref="I63" r:id="rId92" xr:uid="{374CA6C4-4140-5644-83EA-F57344629EA4}"/>
-    <hyperlink ref="I61" r:id="rId93" xr:uid="{2F75C1DE-184C-364D-BCE4-C4C05F05D849}"/>
-    <hyperlink ref="I64" r:id="rId94" xr:uid="{64DD9D18-20A4-7E4D-8427-E81E1D9C2D99}"/>
-    <hyperlink ref="I65" r:id="rId95" xr:uid="{461BD041-D2BF-3846-AF30-4C38F0EF330A}"/>
-    <hyperlink ref="I66" r:id="rId96" xr:uid="{27161EFC-1BEA-C14F-9DDE-D93CCF12DDA2}"/>
-    <hyperlink ref="I67" r:id="rId97" xr:uid="{672EEF39-8D21-2442-A620-17238963188C}"/>
+    <hyperlink ref="J68" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="J21" r:id="rId74" xr:uid="{83A801EE-E546-7444-83B0-7AE4FE5DCC18}"/>
+    <hyperlink ref="J23" r:id="rId75" xr:uid="{6B290F46-1AB5-9544-B3B3-FCE151FC026C}"/>
+    <hyperlink ref="J24" r:id="rId76" xr:uid="{930265A3-4A43-114B-89F7-0D260397ECEE}"/>
+    <hyperlink ref="J25" r:id="rId77" xr:uid="{D7F1F70C-9733-5E46-8B18-FE50DAF1E02B}"/>
+    <hyperlink ref="J26" r:id="rId78" xr:uid="{65733835-2CD9-5749-BBDD-3CBBC33C96FA}"/>
+    <hyperlink ref="J34" r:id="rId79" xr:uid="{5C774A6A-9EAA-6A41-B786-2F3DEE421DF6}"/>
+    <hyperlink ref="J35" r:id="rId80" xr:uid="{1AFAE886-D23A-4C44-9377-F08511F4CB51}"/>
+    <hyperlink ref="J40" r:id="rId81" xr:uid="{04363683-E801-4A40-92D4-F5E22A223193}"/>
+    <hyperlink ref="J41" r:id="rId82" xr:uid="{7765E9B8-43EB-BB45-91B0-4FF8F7D8E3BD}"/>
+    <hyperlink ref="J43" r:id="rId83" xr:uid="{BB0F6366-7063-134D-8A4B-076195A1E08F}"/>
+    <hyperlink ref="J42" r:id="rId84" xr:uid="{DE89AC9B-B4B6-4144-B0BA-3DECB15EAEA2}"/>
+    <hyperlink ref="J46" r:id="rId85" xr:uid="{824B515C-AA87-F043-A139-784BCBF016E6}"/>
+    <hyperlink ref="J49" r:id="rId86" xr:uid="{2AF4CA48-6D36-5947-991C-981DDFA018C7}"/>
+    <hyperlink ref="J50" r:id="rId87" xr:uid="{7056C87E-C05C-9E40-A22A-461D400945D8}"/>
+    <hyperlink ref="J48" r:id="rId88" xr:uid="{7BFDE7F6-5EE7-DB44-9A8C-4A94BA0E0D34}"/>
+    <hyperlink ref="J59" r:id="rId89" xr:uid="{4FE03561-7F01-C941-B63F-6A1C5611F8E0}"/>
+    <hyperlink ref="J60" r:id="rId90" xr:uid="{3EBD3D55-540B-4C48-B378-A997181200FD}"/>
+    <hyperlink ref="J62" r:id="rId91" xr:uid="{3EA893CD-E3C9-F04E-B2E2-7E1A74D042FC}"/>
+    <hyperlink ref="J63" r:id="rId92" xr:uid="{374CA6C4-4140-5644-83EA-F57344629EA4}"/>
+    <hyperlink ref="J61" r:id="rId93" xr:uid="{2F75C1DE-184C-364D-BCE4-C4C05F05D849}"/>
+    <hyperlink ref="J64" r:id="rId94" xr:uid="{64DD9D18-20A4-7E4D-8427-E81E1D9C2D99}"/>
+    <hyperlink ref="J65" r:id="rId95" xr:uid="{461BD041-D2BF-3846-AF30-4C38F0EF330A}"/>
+    <hyperlink ref="J66" r:id="rId96" xr:uid="{27161EFC-1BEA-C14F-9DDE-D93CCF12DDA2}"/>
+    <hyperlink ref="J67" r:id="rId97" xr:uid="{672EEF39-8D21-2442-A620-17238963188C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -61259,7 +61251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A9" s="44">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -61481,7 +61473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="255" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="44">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -61969,7 +61961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="44">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -62074,7 +62066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="221" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -62459,7 +62451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="238" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A43" s="44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -62739,7 +62731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -62774,7 +62766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -62809,7 +62801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -62914,7 +62906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A56" s="44">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -63089,7 +63081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -63630,7 +63622,7 @@
       <c r="J77" s="29"/>
       <c r="K77" s="44"/>
     </row>
-    <row r="78" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="404" x14ac:dyDescent="0.2">
       <c r="A78" s="44">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -63862,7 +63854,7 @@
       <c r="J85" s="29"/>
       <c r="K85" s="44"/>
     </row>
-    <row r="86" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A86" s="44">
         <f t="shared" si="2"/>
         <v>85</v>

</xml_diff>